<commit_message>
Utilized interpolation to account for proper timestep within experimental data. Also utilized interpolation to account for proper offset within pulling experimental data to determine offset for theoretical data
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10_2RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10_2RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\RMSE_Results\E\AngVel\f10_2RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2C9C75-0909-4602-A1D7-1D2DD64A26C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A676B2-1620-4672-A93E-0C409CDD9182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="1092" windowWidth="15120" windowHeight="10788" xr2:uid="{43408AF8-6B8F-4785-94A2-D740DF5006BD}"/>
+    <workbookView xWindow="348" yWindow="1092" windowWidth="15120" windowHeight="10788" xr2:uid="{8AF69D95-9C3D-4986-A67F-398A56F1F7F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076765DC-E3B3-4084-81EC-303CD8441C20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A76EE12-6143-47BF-9656-8BDF0F21629E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Adjusted Mechanism coordinates based from URL (BCEF -> BCFG and CDGI -> CDEI). Also implemeneted positionSolver from PMKS onto MATLAB
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10_2RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10_2RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\RMSE_Results\E\AngVel\f10_2RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9CEC55-6CC2-4801-9AB7-7657993A0CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA228F72-EA5A-402A-8A84-A47866C236A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5148" yWindow="696" windowWidth="15012" windowHeight="10776" xr2:uid="{55B8677B-BD48-4900-9601-BA4B0255FD42}"/>
+    <workbookView xWindow="5256" yWindow="0" windowWidth="14904" windowHeight="10068" xr2:uid="{7AEC915F-F65A-45C0-9689-0060E3393DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,16 +401,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29ACE8D5-7958-43B2-BC33-02D44BA21366}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050EE5B1-557E-4215-A25A-641151DC2F86}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>0.50078020910244514</v>
+        <v>6.3438634657535353E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All the sensors for teaching lab mechanism going 10 rpm now appears to line up ideally
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10_2RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Mechanism/TeachingLab_Four_Bar/RMSE_Results/E/AngVel/f10_2RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Mechanism\TeachingLab_Four_Bar\RMSE_Results\E\AngVel\f10_2RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA228F72-EA5A-402A-8A84-A47866C236A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A3D4B8-B099-4713-AD25-F7363E517914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5256" yWindow="0" windowWidth="14904" windowHeight="10068" xr2:uid="{7AEC915F-F65A-45C0-9689-0060E3393DB1}"/>
+    <workbookView xWindow="5256" yWindow="0" windowWidth="14904" windowHeight="10068" xr2:uid="{D10CBBB1-B30F-4DDA-8CD8-1826F39E2E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050EE5B1-557E-4215-A25A-641151DC2F86}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEB3695-C96D-4195-8BCF-5D68EE4C0A73}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>